<commit_message>
cambios de idioma a events, route, stops, summary, trips
</commit_message>
<xml_diff>
--- a/templates/export/route.xlsx
+++ b/templates/export/route.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_2A0B9F050BF4C803F7395527D93F516D8924CED2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA5A2FA8-DB2D-48DD-A083-DC25CB9FEBBB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Автор</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -38,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -73,51 +74,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>Report type:</t>
-  </si>
-  <si>
-    <t>Route</t>
-  </si>
-  <si>
-    <t>Device:</t>
-  </si>
-  <si>
     <t>${device.deviceName}</t>
   </si>
   <si>
-    <t>Group:</t>
-  </si>
-  <si>
     <t>${device.groupName}</t>
   </si>
   <si>
-    <t>Period:</t>
-  </si>
-  <si>
-    <t>Valid</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Altitude</t>
-  </si>
-  <si>
-    <t>Speed</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Attributes</t>
-  </si>
-  <si>
     <t>${position.valid}</t>
   </si>
   <si>
@@ -143,12 +105,51 @@
   </si>
   <si>
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", position.fixTime, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>Tipo de Reporte:</t>
+  </si>
+  <si>
+    <t>Ruta</t>
+  </si>
+  <si>
+    <t>Dispositivo:</t>
+  </si>
+  <si>
+    <t>Grupo:</t>
+  </si>
+  <si>
+    <t>Periodo:</t>
+  </si>
+  <si>
+    <t>Validación</t>
+  </si>
+  <si>
+    <t>Tiempo</t>
+  </si>
+  <si>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
+  <si>
+    <t>Altitud</t>
+  </si>
+  <si>
+    <t>Velocidad</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>Atributos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -285,7 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -293,14 +294,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -342,8 +342,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Пояснение" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -437,13 +437,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4019040</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:colOff>3761865</xdr:colOff>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -488,13 +494,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4019040</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:colOff>3761865</xdr:colOff>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -539,13 +551,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>4019040</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:colOff>3761865</xdr:colOff>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -596,7 +614,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -639,7 +663,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -682,7 +712,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -975,16 +1011,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.7109375"/>
     <col min="3" max="4" width="13"/>
     <col min="5" max="5" width="10.7109375"/>
@@ -997,139 +1033,112 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
+      <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="18" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>